<commit_message>
Updated DigitalDownloadsExecution.java DigitalDownloadsPage.java ExcelData.xlsx
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace-DWS\DemoWebShopDWS_Taf\DemoWebShopDWS_Taf\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99219F9A-E8F6-4502-A8C7-2FA6380DAD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16710" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>TestCase</t>
   </si>
@@ -75,9 +69,6 @@
     <t>meghadevaraja1998@gmail.com</t>
   </si>
   <si>
-    <t>DigitalDownloadsExecution.checkout</t>
-  </si>
-  <si>
     <t>New Address</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>Devaraj</t>
   </si>
   <si>
-    <t>meghadmeghad@gmail.com</t>
-  </si>
-  <si>
     <t>Bengaluru</t>
   </si>
   <si>
@@ -135,15 +123,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Entered FirstName</t>
-  </si>
-  <si>
-    <t>Entered LastName</t>
-  </si>
-  <si>
-    <t>Entered Email</t>
-  </si>
-  <si>
     <t>BooksExecution.booksPageTest</t>
   </si>
   <si>
@@ -301,13 +280,19 @@
   </si>
   <si>
     <t>Assertion21</t>
+  </si>
+  <si>
+    <t>meghadmegha@gmail.com</t>
+  </si>
+  <si>
+    <t>DigitalDownloadsExecution.digitalDownloads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,48 +658,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" customWidth="1"/>
-    <col min="9" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" customWidth="1"/>
-    <col min="14" max="14" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
     <col min="15" max="15" width="28" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="13.5546875" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
     <col min="18" max="18" width="25" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
-    <col min="20" max="20" width="23.21875" customWidth="1"/>
-    <col min="21" max="21" width="15.88671875" customWidth="1"/>
-    <col min="22" max="22" width="16.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" customWidth="1"/>
-    <col min="24" max="24" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="23.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -725,34 +710,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>7</v>
@@ -773,56 +758,56 @@
         <v>8</v>
       </c>
       <c r="T1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -830,7 +815,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -868,7 +853,7 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -914,32 +899,32 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="K4" s="3">
         <v>560085</v>
@@ -948,31 +933,41 @@
         <v>9874563321</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" s="3">
+        <v>560085</v>
+      </c>
+      <c r="W4" s="3">
+        <v>9874563321</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
@@ -986,32 +981,32 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K5" s="3">
         <v>560085</v>
@@ -1020,10 +1015,10 @@
         <v>9019139736</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1048,36 +1043,36 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3">
         <v>131099</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K6" s="4">
         <v>560085</v>
@@ -1086,22 +1081,22 @@
         <v>7829508059</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P6" s="1">
         <v>131099</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1122,32 +1117,32 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K7" s="3">
         <v>560032</v>
@@ -1156,10 +1151,10 @@
         <v>9735553204</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1184,32 +1179,32 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K8" s="3">
         <v>560085</v>
@@ -1218,10 +1213,10 @@
         <v>7892540781</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1246,32 +1241,32 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K9" s="3">
         <v>560096</v>
@@ -1280,10 +1275,10 @@
         <v>7411313729</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1308,32 +1303,32 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K10" s="3">
         <v>560085</v>
@@ -1342,10 +1337,10 @@
         <v>7019561257</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1373,33 +1368,30 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="H8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="H9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="H10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B4" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C4" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C2" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="O6" r:id="rId24" xr:uid="{784FE630-B003-4898-B6CE-A2111F3518C7}"/>
-    <hyperlink ref="R6" r:id="rId25" xr:uid="{2CE85286-3F6D-4EAC-BB42-49A763F67E15}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="H7" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="H5" r:id="rId8"/>
+    <hyperlink ref="B8" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="H8" r:id="rId11"/>
+    <hyperlink ref="B9" r:id="rId12"/>
+    <hyperlink ref="C9" r:id="rId13"/>
+    <hyperlink ref="H9" r:id="rId14"/>
+    <hyperlink ref="B10" r:id="rId15"/>
+    <hyperlink ref="C10" r:id="rId16"/>
+    <hyperlink ref="H10" r:id="rId17"/>
+    <hyperlink ref="B6" r:id="rId18"/>
+    <hyperlink ref="H6" r:id="rId19"/>
+    <hyperlink ref="C2" r:id="rId20"/>
+    <hyperlink ref="O6" r:id="rId21"/>
+    <hyperlink ref="R6" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Automation Script on ComputerExecution.java and ExcelData.xlsx
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16710" windowHeight="6540"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="16524" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>TestCase</t>
   </si>
@@ -69,6 +69,9 @@
     <t>meghadevaraja1998@gmail.com</t>
   </si>
   <si>
+    <t>DigitalDownloadsExecution.checkout</t>
+  </si>
+  <si>
     <t>New Address</t>
   </si>
   <si>
@@ -114,6 +117,9 @@
     <t>Devaraj</t>
   </si>
   <si>
+    <t>meghadmeghad@gmail.com</t>
+  </si>
+  <si>
     <t>Bengaluru</t>
   </si>
   <si>
@@ -123,6 +129,15 @@
     <t>India</t>
   </si>
   <si>
+    <t>Entered FirstName</t>
+  </si>
+  <si>
+    <t>Entered LastName</t>
+  </si>
+  <si>
+    <t>Entered Email</t>
+  </si>
+  <si>
     <t>BooksExecution.booksPageTest</t>
   </si>
   <si>
@@ -282,17 +297,14 @@
     <t>Assertion21</t>
   </si>
   <si>
-    <t>meghadmegha@gmail.com</t>
-  </si>
-  <si>
-    <t>DigitalDownloadsExecution.digitalDownloads</t>
+    <t>kattriguppe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +338,12 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,7 +385,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -385,6 +403,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -668,35 +687,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" customWidth="1"/>
+    <col min="9" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" customWidth="1"/>
     <col min="15" max="15" width="28" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" customWidth="1"/>
-    <col min="18" max="18" width="25" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" customWidth="1"/>
+    <col min="17" max="17" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.77734375" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.21875" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.21875" customWidth="1"/>
+    <col min="24" max="24" width="20" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -710,34 +730,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>7</v>
@@ -758,52 +778,52 @@
         <v>8</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="AI1" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="AJ1" s="1"/>
     </row>
@@ -815,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -901,30 +921,30 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" s="3">
         <v>560085</v>
@@ -933,41 +953,31 @@
         <v>9874563321</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" s="3">
-        <v>560085</v>
-      </c>
-      <c r="W4" s="3">
-        <v>9874563321</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
@@ -983,30 +993,30 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="K5" s="3">
         <v>560085</v>
@@ -1015,22 +1025,44 @@
         <v>9019139736</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X5" s="1">
+        <v>560085</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>9019139736</v>
+      </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
@@ -1045,34 +1077,34 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3">
         <v>131099</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="K6" s="4">
         <v>560085</v>
@@ -1081,22 +1113,22 @@
         <v>7829508059</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P6" s="1">
         <v>131099</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1119,30 +1151,30 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="K7" s="3">
         <v>560032</v>
@@ -1151,10 +1183,10 @@
         <v>9735553204</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1181,30 +1213,30 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K8" s="3">
         <v>560085</v>
@@ -1213,10 +1245,10 @@
         <v>7892540781</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1243,30 +1275,30 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="K9" s="3">
         <v>560096</v>
@@ -1275,10 +1307,10 @@
         <v>7411313729</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1305,30 +1337,30 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K10" s="3">
         <v>560085</v>
@@ -1337,13 +1369,15 @@
         <v>7019561257</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -1371,27 +1405,34 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="H7" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="H5" r:id="rId8"/>
-    <hyperlink ref="B8" r:id="rId9"/>
-    <hyperlink ref="C8" r:id="rId10"/>
-    <hyperlink ref="H8" r:id="rId11"/>
-    <hyperlink ref="B9" r:id="rId12"/>
-    <hyperlink ref="C9" r:id="rId13"/>
-    <hyperlink ref="H9" r:id="rId14"/>
-    <hyperlink ref="B10" r:id="rId15"/>
-    <hyperlink ref="C10" r:id="rId16"/>
-    <hyperlink ref="H10" r:id="rId17"/>
-    <hyperlink ref="B6" r:id="rId18"/>
-    <hyperlink ref="H6" r:id="rId19"/>
-    <hyperlink ref="C2" r:id="rId20"/>
-    <hyperlink ref="O6" r:id="rId21"/>
-    <hyperlink ref="R6" r:id="rId22"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId8"/>
+    <hyperlink ref="H5" r:id="rId9"/>
+    <hyperlink ref="B8" r:id="rId10"/>
+    <hyperlink ref="C8" r:id="rId11"/>
+    <hyperlink ref="H8" r:id="rId12"/>
+    <hyperlink ref="B9" r:id="rId13"/>
+    <hyperlink ref="C9" r:id="rId14"/>
+    <hyperlink ref="H9" r:id="rId15"/>
+    <hyperlink ref="B10" r:id="rId16"/>
+    <hyperlink ref="C10" r:id="rId17"/>
+    <hyperlink ref="H10" r:id="rId18"/>
+    <hyperlink ref="B6" r:id="rId19"/>
+    <hyperlink ref="H6" r:id="rId20"/>
+    <hyperlink ref="B4" r:id="rId21"/>
+    <hyperlink ref="C4" r:id="rId22"/>
+    <hyperlink ref="C2" r:id="rId23"/>
+    <hyperlink ref="O6" r:id="rId24"/>
+    <hyperlink ref="R6" r:id="rId25"/>
+    <hyperlink ref="P10" r:id="rId26"/>
+    <hyperlink ref="P5" r:id="rId27"/>
+    <hyperlink ref="S5" r:id="rId28" display="lalipreeti9@gmail.com"/>
+    <hyperlink ref="T5" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel data for my 6th row and updated my test case GiftcardsExceution.java and Updated HomePageDWS because jewellery menu xpath had one extra bracket in xpath
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace-DWS\DemoWebShopDWS_Taf\DemoWebShopDWS_Taf\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770F6E15-1CA1-4E70-83B0-D0EBE219E3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="16524" windowHeight="8220"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>TestCase</t>
   </si>
@@ -303,8 +309,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,7 +391,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -404,6 +410,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -677,21 +685,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Z11" activeCellId="1" sqref="Q6 Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.88671875" customWidth="1"/>
@@ -712,14 +720,14 @@
     <col min="18" max="18" width="22.77734375" customWidth="1"/>
     <col min="19" max="19" width="20.6640625" customWidth="1"/>
     <col min="20" max="20" width="23.21875" customWidth="1"/>
-    <col min="21" max="21" width="15.88671875" customWidth="1"/>
+    <col min="21" max="21" width="25.33203125" customWidth="1"/>
     <col min="22" max="22" width="16.6640625" customWidth="1"/>
     <col min="23" max="23" width="15.21875" customWidth="1"/>
     <col min="24" max="24" width="20" customWidth="1"/>
     <col min="25" max="25" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -827,7 +835,7 @@
       </c>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -873,7 +881,7 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -919,7 +927,7 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -991,7 +999,7 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1075,35 +1083,35 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="1:36">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <v>131099</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="10" t="s">
         <v>73</v>
       </c>
       <c r="K6" s="4">
@@ -1112,44 +1120,58 @@
       <c r="L6" s="4">
         <v>7829508059</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="3">
         <v>131099</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
+      <c r="S6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6" s="2">
+        <v>560085</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>7829508059</v>
+      </c>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1211,7 +1233,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1273,7 +1295,7 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -1335,7 +1357,7 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1402,37 +1424,38 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="H4" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="B5" r:id="rId7"/>
-    <hyperlink ref="C5" r:id="rId8"/>
-    <hyperlink ref="H5" r:id="rId9"/>
-    <hyperlink ref="B8" r:id="rId10"/>
-    <hyperlink ref="C8" r:id="rId11"/>
-    <hyperlink ref="H8" r:id="rId12"/>
-    <hyperlink ref="B9" r:id="rId13"/>
-    <hyperlink ref="C9" r:id="rId14"/>
-    <hyperlink ref="H9" r:id="rId15"/>
-    <hyperlink ref="B10" r:id="rId16"/>
-    <hyperlink ref="C10" r:id="rId17"/>
-    <hyperlink ref="H10" r:id="rId18"/>
-    <hyperlink ref="B6" r:id="rId19"/>
-    <hyperlink ref="H6" r:id="rId20"/>
-    <hyperlink ref="B4" r:id="rId21"/>
-    <hyperlink ref="C4" r:id="rId22"/>
-    <hyperlink ref="C2" r:id="rId23"/>
-    <hyperlink ref="O6" r:id="rId24"/>
-    <hyperlink ref="R6" r:id="rId25"/>
-    <hyperlink ref="P10" r:id="rId26"/>
-    <hyperlink ref="P5" r:id="rId27"/>
-    <hyperlink ref="S5" r:id="rId28" display="lalipreeti9@gmail.com"/>
-    <hyperlink ref="T5" r:id="rId29"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B4" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C4" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C2" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="O6" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="R6" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="P10" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="P5" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="S5" r:id="rId28" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="T5" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="U6" r:id="rId30" xr:uid="{8BC5952A-ADEF-4030-B9A4-294426D2B8C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Automation Test script on BooksPage.java,BooksExecution.java and ExcelData.xlsx
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MQAS_ETL_SEPT2022\Workspace_DWS\DemoWebShop-taf\DemoWebShopDWS_Taf\git\DemoWebShopDWS_Taf\DemoWebShopDWS_Taf\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F1AAC7-4E2F-454C-8811-F4B2345DF041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
   <si>
     <t>TestCase</t>
   </si>
@@ -294,8 +300,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,49 +676,49 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" customWidth="1"/>
+    <col min="9" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" customWidth="1"/>
     <col min="15" max="15" width="28" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="23.28515625" customWidth="1"/>
-    <col min="21" max="21" width="25.28515625" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" customWidth="1"/>
+    <col min="21" max="21" width="25.33203125" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" customWidth="1"/>
     <col min="24" max="24" width="20" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -820,7 +826,7 @@
       </c>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -866,7 +872,7 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -912,7 +918,7 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -992,7 +998,7 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1076,7 +1082,7 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="1:36" s="11" customFormat="1">
+    <row r="6" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
@@ -1164,7 +1170,7 @@
       <c r="AI6" s="10"/>
       <c r="AJ6" s="10"/>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1203,16 +1209,36 @@
       <c r="N7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
+      <c r="O7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="3">
+        <v>560032</v>
+      </c>
+      <c r="W7" s="3">
+        <v>9735553204</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -1226,7 +1252,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1288,7 +1314,7 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1350,7 +1376,7 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
@@ -1417,35 +1443,37 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="H7" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="H5" r:id="rId8"/>
-    <hyperlink ref="B8" r:id="rId9"/>
-    <hyperlink ref="C8" r:id="rId10"/>
-    <hyperlink ref="H8" r:id="rId11"/>
-    <hyperlink ref="B9" r:id="rId12"/>
-    <hyperlink ref="C9" r:id="rId13"/>
-    <hyperlink ref="H9" r:id="rId14"/>
-    <hyperlink ref="B10" r:id="rId15"/>
-    <hyperlink ref="C10" r:id="rId16"/>
-    <hyperlink ref="H10" r:id="rId17"/>
-    <hyperlink ref="B6" r:id="rId18"/>
-    <hyperlink ref="H6" r:id="rId19"/>
-    <hyperlink ref="C2" r:id="rId20"/>
-    <hyperlink ref="O6" r:id="rId21"/>
-    <hyperlink ref="R6" r:id="rId22"/>
-    <hyperlink ref="P10" r:id="rId23"/>
-    <hyperlink ref="P5" r:id="rId24"/>
-    <hyperlink ref="S5" r:id="rId25" display="lalipreeti9@gmail.com"/>
-    <hyperlink ref="T5" r:id="rId26"/>
-    <hyperlink ref="U6" r:id="rId27"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B6" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H6" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="O6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="R6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="P10" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="P5" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="S5" r:id="rId23" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="T5" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="U6" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B7" r:id="rId26" xr:uid="{8C399F61-DB76-4FD2-979E-30DA4A7214C1}"/>
+    <hyperlink ref="H7" r:id="rId27" xr:uid="{83F25A73-E7BA-418C-80CA-2B2C48E92AA6}"/>
+    <hyperlink ref="O7" r:id="rId28" xr:uid="{13568ADE-F311-42B5-8C57-0ACADB56D5A5}"/>
+    <hyperlink ref="S7" r:id="rId29" xr:uid="{FC134E99-CD2A-4DA5-B3E0-D48980B830B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Jewelry script is added
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MQAS_ETL_SEPT2022\Workspace_DWS\DemoWebShop-taf\DemoWebShopDWS_Taf\git\DemoWebShopDWS_Taf\DemoWebShopDWS_Taf\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MQAS Batch\Workspace DWS\DemoWebShop-taf\git\DemoWebShopDWS_Taf\DemoWebShopDWS_Taf\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F1AAC7-4E2F-454C-8811-F4B2345DF041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>TestCase</t>
   </si>
@@ -183,9 +182,6 @@
     <t>SM</t>
   </si>
   <si>
-    <t>JewelryExecution.chekout</t>
-  </si>
-  <si>
     <t>vanigowdas54@gmail.com</t>
   </si>
   <si>
@@ -295,12 +291,15 @@
   </si>
   <si>
     <t>DigitalDownloadsExecution.digitalDownloads</t>
+  </si>
+  <si>
+    <t>JewelryExecution.checkout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -683,11 +682,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +755,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>7</v>
@@ -777,52 +776,52 @@
         <v>8</v>
       </c>
       <c r="T1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="AJ1" s="1"/>
     </row>
@@ -834,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -920,13 +919,13 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1023,7 +1022,7 @@
         <v>46</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K5" s="3">
         <v>560085</v>
@@ -1062,7 +1061,7 @@
         <v>46</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X5" s="1">
         <v>560085</v>
@@ -1087,7 +1086,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="10">
         <v>131099</v>
@@ -1099,19 +1098,19 @@
         <v>21</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="K6" s="4">
         <v>560085</v>
@@ -1126,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P6" s="3">
         <v>131099</v>
@@ -1138,19 +1137,19 @@
         <v>21</v>
       </c>
       <c r="S6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="U6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="V6" s="10" t="s">
+      <c r="W6" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="X6" s="2">
         <v>560085</v>
@@ -1316,30 +1315,30 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K9" s="3">
         <v>560096</v>
@@ -1353,16 +1352,34 @@
       <c r="N9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="O9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
+      <c r="U9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W9" s="1">
+        <v>560096</v>
+      </c>
+      <c r="X9" s="1">
+        <v>7411313729</v>
+      </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -1378,30 +1395,30 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="3">
         <v>560085</v>
@@ -1443,37 +1460,42 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="H8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="H9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="H10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B6" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="H6" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="O6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="R6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="P10" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="P5" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="S5" r:id="rId23" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="T5" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="U6" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B7" r:id="rId26" xr:uid="{8C399F61-DB76-4FD2-979E-30DA4A7214C1}"/>
-    <hyperlink ref="H7" r:id="rId27" xr:uid="{83F25A73-E7BA-418C-80CA-2B2C48E92AA6}"/>
-    <hyperlink ref="O7" r:id="rId28" xr:uid="{13568ADE-F311-42B5-8C57-0ACADB56D5A5}"/>
-    <hyperlink ref="S7" r:id="rId29" xr:uid="{FC134E99-CD2A-4DA5-B3E0-D48980B830B6}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="H5" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
+    <hyperlink ref="H8" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="C9" r:id="rId11"/>
+    <hyperlink ref="H9" r:id="rId12"/>
+    <hyperlink ref="B10" r:id="rId13"/>
+    <hyperlink ref="C10" r:id="rId14"/>
+    <hyperlink ref="H10" r:id="rId15"/>
+    <hyperlink ref="B6" r:id="rId16"/>
+    <hyperlink ref="H6" r:id="rId17"/>
+    <hyperlink ref="C2" r:id="rId18"/>
+    <hyperlink ref="O6" r:id="rId19"/>
+    <hyperlink ref="R6" r:id="rId20"/>
+    <hyperlink ref="P10" r:id="rId21"/>
+    <hyperlink ref="P5" r:id="rId22"/>
+    <hyperlink ref="S5" r:id="rId23" display="lalipreeti9@gmail.com"/>
+    <hyperlink ref="T5" r:id="rId24"/>
+    <hyperlink ref="U6" r:id="rId25"/>
+    <hyperlink ref="B7" r:id="rId26"/>
+    <hyperlink ref="H7" r:id="rId27"/>
+    <hyperlink ref="O7" r:id="rId28"/>
+    <hyperlink ref="S7" r:id="rId29"/>
+    <hyperlink ref="O9" r:id="rId30"/>
+    <hyperlink ref="P9" r:id="rId31"/>
+    <hyperlink ref="Q9" r:id="rId32" display="Vanigowdas54@gmail.com"/>
+    <hyperlink ref="R9" r:id="rId33" display="meghadmeghad@gmail.com"/>
+    <hyperlink ref="S9" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel Data--Added Columns
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E230A-A77F-4C91-AA92-80EF597F03AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>TestCase</t>
   </si>
@@ -247,13 +248,19 @@
   </si>
   <si>
     <t>JewelryExecution.checkout</t>
+  </si>
+  <si>
+    <t>Username-Assertion</t>
+  </si>
+  <si>
+    <t>Password-Assertion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,7 +356,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -371,11 +378,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,6 +388,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -429,7 +442,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,9 +474,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,6 +526,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -670,20 +719,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="1" max="1" width="41.21875" customWidth="1"/>
+    <col min="2" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="20.5546875" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.88671875" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="21.44140625" customWidth="1"/>
+    <col min="21" max="21" width="24" customWidth="1"/>
+    <col min="22" max="22" width="24.5546875" customWidth="1"/>
+    <col min="23" max="23" width="29" customWidth="1"/>
+    <col min="24" max="24" width="17.88671875" customWidth="1"/>
+    <col min="25" max="25" width="16.88671875" customWidth="1"/>
+    <col min="26" max="26" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="4" customFormat="1">
+    <row r="1" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,64 +762,68 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
@@ -769,36 +844,38 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:43" s="8" customFormat="1">
+    <row r="2" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
@@ -821,37 +898,39 @@
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:43" s="8" customFormat="1">
+    <row r="3" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
+      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="6"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="9"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
@@ -873,73 +952,75 @@
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
       <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:43" s="8" customFormat="1">
+    <row r="4" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="7">
+      <c r="T4" s="7">
         <v>560085</v>
       </c>
-      <c r="S4" s="5">
+      <c r="U4" s="5">
         <v>560085</v>
       </c>
-      <c r="T4" s="5">
+      <c r="V4" s="5">
         <v>9874563210</v>
       </c>
-      <c r="U4" s="5">
+      <c r="W4" s="5">
         <v>9874563210</v>
       </c>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
@@ -959,81 +1040,83 @@
       <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
       <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="13">
+      <c r="M5" s="13">
         <v>560085</v>
       </c>
-      <c r="L5" s="13">
+      <c r="N5" s="13">
         <v>9019139736</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="R5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="T5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="U5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="V5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="W5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="X5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="Y5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="X5" s="11">
+      <c r="Z5" s="11">
         <v>560085</v>
       </c>
-      <c r="Y5" s="11">
+      <c r="AA5" s="11">
         <v>9019139736</v>
       </c>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
@@ -1043,166 +1126,174 @@
       <c r="AH5" s="11"/>
       <c r="AI5" s="11"/>
       <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
     </row>
-    <row r="6" spans="1:43" s="17" customFormat="1">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="11">
         <v>131099</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="11">
+        <v>131099</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="15">
+        <v>560085</v>
+      </c>
+      <c r="N6" s="15">
+        <v>7829508059</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="13">
+        <v>131099</v>
+      </c>
+      <c r="S6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="T6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="U6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="V6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="W6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="X6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="Y6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="16">
+      <c r="Z6" s="12">
         <v>560085</v>
       </c>
-      <c r="L6" s="16">
+      <c r="AA6" s="12">
         <v>7829508059</v>
       </c>
-      <c r="M6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="13">
-        <v>131099</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="R6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="T6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="W6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="X6" s="12">
-        <v>560085</v>
-      </c>
-      <c r="Y6" s="12">
-        <v>7829508059</v>
-      </c>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="13">
+      <c r="M7" s="13">
         <v>560032</v>
       </c>
-      <c r="L7" s="13">
+      <c r="N7" s="13">
         <v>9735553204</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="O7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="P7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="R7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="S7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="T7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="U7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="T7" s="11" t="s">
+      <c r="V7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="U7" s="11" t="s">
+      <c r="W7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="V7" s="13">
+      <c r="X7" s="13">
         <v>560032</v>
       </c>
-      <c r="W7" s="13">
+      <c r="Y7" s="13">
         <v>9735553204</v>
       </c>
-      <c r="X7" s="11" t="s">
+      <c r="Z7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
@@ -1213,48 +1304,50 @@
       <c r="AH7" s="11"/>
       <c r="AI7" s="11"/>
       <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="J8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="13">
+      <c r="M8" s="13">
         <v>560085</v>
       </c>
-      <c r="L8" s="13">
+      <c r="N8" s="13">
         <v>7892540781</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
@@ -1275,48 +1368,50 @@
       <c r="AH8" s="11"/>
       <c r="AI8" s="11"/>
       <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>76</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="J9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="L9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="13">
+      <c r="M9" s="13">
         <v>560096</v>
       </c>
-      <c r="L9" s="13">
+      <c r="N9" s="13">
         <v>7411313729</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="O9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
@@ -1337,52 +1432,54 @@
       <c r="AH9" s="11"/>
       <c r="AI9" s="11"/>
       <c r="AJ9" s="11"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="11"/>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="J10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="L10" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K10" s="13">
+      <c r="M10" s="13">
         <v>560085</v>
       </c>
-      <c r="L10" s="13">
+      <c r="N10" s="13">
         <v>7019561257</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="O10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="P10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12" t="s">
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
       <c r="U10" s="11"/>
@@ -1401,62 +1498,64 @@
       <c r="AH10" s="11"/>
       <c r="AI10" s="11"/>
       <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="C9" r:id="rId9"/>
-    <hyperlink ref="H9" r:id="rId10"/>
-    <hyperlink ref="B10" r:id="rId11"/>
-    <hyperlink ref="C10" r:id="rId12"/>
-    <hyperlink ref="H10" r:id="rId13"/>
-    <hyperlink ref="B6" r:id="rId14"/>
-    <hyperlink ref="H6" r:id="rId15"/>
-    <hyperlink ref="O6" r:id="rId16"/>
-    <hyperlink ref="R6" r:id="rId17"/>
-    <hyperlink ref="P10" r:id="rId18"/>
-    <hyperlink ref="P5" r:id="rId19"/>
-    <hyperlink ref="S5" r:id="rId20" display="lalipreeti9@gmail.com"/>
-    <hyperlink ref="T5" r:id="rId21"/>
-    <hyperlink ref="U6" r:id="rId22"/>
-    <hyperlink ref="B7" r:id="rId23"/>
-    <hyperlink ref="H7" r:id="rId24"/>
-    <hyperlink ref="O7" r:id="rId25"/>
-    <hyperlink ref="S7" r:id="rId26"/>
-    <hyperlink ref="B3" r:id="rId27" display="Bharathkumar@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId28" display="lalipreeti9@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId29" display="PreetiLali@123"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="Q6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="T6" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="R10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="R5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="U5" r:id="rId19" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="V5" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="W6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="Q7" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="U7" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B3" r:id="rId26" display="Bharathkumar@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B2" r:id="rId27" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D2" r:id="rId28" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C6" r:id="rId29" xr:uid="{018D9D79-8408-4586-BFE2-D05DD6804DF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Jewelry script is updated
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C036E765-5366-45D5-83DA-35E7AD2150AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>TestCase</t>
   </si>
@@ -259,7 +258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,23 +477,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -530,23 +512,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,47 +1346,69 @@
       <c r="B9" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="E9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="H9" s="11" t="s">
         <v>66</v>
       </c>
       <c r="I9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="K9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="13">
-        <v>560096</v>
-      </c>
-      <c r="N9" s="13">
-        <v>7411313729</v>
+      <c r="M9" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="O9" s="11" t="s">
         <v>34</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="T9" s="11">
+        <v>560096</v>
+      </c>
+      <c r="U9" s="11">
+        <v>560096</v>
+      </c>
+      <c r="V9" s="11">
+        <v>7411313729</v>
+      </c>
+      <c r="W9" s="11">
+        <v>7411313729</v>
+      </c>
       <c r="X9" s="11"/>
       <c r="Y9" s="11"/>
       <c r="Z9" s="11"/>
@@ -1506,42 +1493,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="J8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="J6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="Q6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="T6" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="R10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="R5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="U5" r:id="rId19" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="V5" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="W6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="J7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="Q7" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="U7" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B3" r:id="rId26" display="Bharathkumar@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B2" r:id="rId27" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D2" r:id="rId28" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C6" r:id="rId29" xr:uid="{8BD0FA59-97CC-4118-B9A3-77987A49C939}"/>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="J5" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="J8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="D10" r:id="rId10"/>
+    <hyperlink ref="J10" r:id="rId11"/>
+    <hyperlink ref="B6" r:id="rId12"/>
+    <hyperlink ref="J6" r:id="rId13"/>
+    <hyperlink ref="Q6" r:id="rId14"/>
+    <hyperlink ref="T6" r:id="rId15"/>
+    <hyperlink ref="R10" r:id="rId16"/>
+    <hyperlink ref="R5" r:id="rId17"/>
+    <hyperlink ref="U5" r:id="rId18" display="lalipreeti9@gmail.com"/>
+    <hyperlink ref="V5" r:id="rId19"/>
+    <hyperlink ref="W6" r:id="rId20"/>
+    <hyperlink ref="B7" r:id="rId21"/>
+    <hyperlink ref="J7" r:id="rId22"/>
+    <hyperlink ref="Q7" r:id="rId23"/>
+    <hyperlink ref="U7" r:id="rId24"/>
+    <hyperlink ref="B3" r:id="rId25" display="Bharathkumar@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId26" display="lalipreeti9@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId27" display="PreetiLali@123"/>
+    <hyperlink ref="C6" r:id="rId28"/>
+    <hyperlink ref="C9" r:id="rId29"/>
+    <hyperlink ref="E9" r:id="rId30"/>
+    <hyperlink ref="L9" r:id="rId31"/>
+    <hyperlink ref="M9" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1553,7 +1543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated BooksExecution.java Script and ExcelData
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143B54FB-3027-4E48-B505-EF8E9D1F4C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="79">
   <si>
     <t>TestCase</t>
   </si>
@@ -258,8 +259,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,7 +445,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -476,9 +477,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -510,6 +529,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -685,42 +722,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.5546875" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.88671875" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
     <col min="18" max="18" width="17" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" customWidth="1"/>
-    <col min="20" max="20" width="21.42578125" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="21.44140625" customWidth="1"/>
     <col min="21" max="21" width="24" customWidth="1"/>
-    <col min="22" max="22" width="24.5703125" customWidth="1"/>
+    <col min="22" max="22" width="24.5546875" customWidth="1"/>
     <col min="23" max="23" width="29" customWidth="1"/>
-    <col min="24" max="24" width="17.85546875" customWidth="1"/>
-    <col min="25" max="25" width="16.85546875" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" customWidth="1"/>
+    <col min="24" max="24" width="17.88671875" customWidth="1"/>
+    <col min="25" max="25" width="16.88671875" customWidth="1"/>
+    <col min="26" max="26" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="4" customFormat="1">
+    <row r="1" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +850,7 @@
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:45" s="8" customFormat="1">
+    <row r="2" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -867,7 +904,7 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:45" s="8" customFormat="1">
+    <row r="3" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -921,7 +958,7 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:45" s="8" customFormat="1">
+    <row r="4" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1009,7 +1046,7 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>37</v>
       </c>
@@ -1095,7 +1132,7 @@
       <c r="AK5" s="11"/>
       <c r="AL5" s="11"/>
     </row>
-    <row r="6" spans="1:45" s="16" customFormat="1">
+    <row r="6" spans="1:45" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
@@ -1189,77 +1226,79 @@
       <c r="AK6" s="13"/>
       <c r="AL6" s="13"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="D7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="H7" s="11" t="s">
         <v>55</v>
       </c>
       <c r="I7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="K7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" s="13">
-        <v>560032</v>
-      </c>
-      <c r="N7" s="13">
-        <v>9735553204</v>
+      <c r="M7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="O7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>53</v>
+      <c r="P7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="W7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="X7" s="13">
+      <c r="T7" s="11">
         <v>560032</v>
       </c>
-      <c r="Y7" s="13">
-        <v>9735553204</v>
-      </c>
-      <c r="Z7" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="U7" s="11">
+        <v>560032</v>
+      </c>
+      <c r="V7" s="11">
+        <v>9735864256</v>
+      </c>
+      <c r="W7" s="11">
+        <v>9735864256</v>
+      </c>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
@@ -1273,7 +1312,7 @@
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
@@ -1337,7 +1376,7 @@
       <c r="AK8" s="11"/>
       <c r="AL8" s="11"/>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>75</v>
       </c>
@@ -1423,7 +1462,7 @@
       <c r="AK9" s="11"/>
       <c r="AL9" s="11"/>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>70</v>
       </c>
@@ -1511,42 +1550,43 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="J5" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="J8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="D10" r:id="rId10"/>
-    <hyperlink ref="J10" r:id="rId11" display="pinkypriya@123gmail.com"/>
-    <hyperlink ref="B6" r:id="rId12"/>
-    <hyperlink ref="J6" r:id="rId13"/>
-    <hyperlink ref="Q6" r:id="rId14"/>
-    <hyperlink ref="T6" r:id="rId15"/>
-    <hyperlink ref="R10" r:id="rId16" display="PreetiLali@123"/>
-    <hyperlink ref="R5" r:id="rId17"/>
-    <hyperlink ref="U5" r:id="rId18" display="lalipreeti9@gmail.com"/>
-    <hyperlink ref="V5" r:id="rId19"/>
-    <hyperlink ref="W6" r:id="rId20"/>
-    <hyperlink ref="B7" r:id="rId21"/>
-    <hyperlink ref="J7" r:id="rId22"/>
-    <hyperlink ref="Q7" r:id="rId23"/>
-    <hyperlink ref="U7" r:id="rId24"/>
-    <hyperlink ref="B3" r:id="rId25" display="Bharathkumar@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId26" display="lalipreeti9@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId27" display="PreetiLali@123"/>
-    <hyperlink ref="C6" r:id="rId28"/>
-    <hyperlink ref="C9" r:id="rId29"/>
-    <hyperlink ref="E9" r:id="rId30"/>
-    <hyperlink ref="L9" r:id="rId31"/>
-    <hyperlink ref="M9" r:id="rId32"/>
-    <hyperlink ref="C10" r:id="rId33"/>
-    <hyperlink ref="E10" r:id="rId34"/>
-    <hyperlink ref="L10" r:id="rId35"/>
-    <hyperlink ref="M10" r:id="rId36"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J10" r:id="rId11" display="pinkypriya@123gmail.com" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B6" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="Q6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="T6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="R10" r:id="rId16" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="R5" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="U5" r:id="rId18" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="V5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="W6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B3" r:id="rId21" display="Bharathkumar@gmail.com" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B2" r:id="rId22" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D2" r:id="rId23" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C6" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C9" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E9" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="L9" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M9" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C10" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E10" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="L10" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="M10" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B7" r:id="rId33" xr:uid="{6F948A64-9E9A-489A-AAC1-1176D705DD43}"/>
+    <hyperlink ref="J7" r:id="rId34" display="tejaswinirty@gmail.com" xr:uid="{5A114D6A-FC17-4BA0-8D32-E28FC2B09E9A}"/>
+    <hyperlink ref="C7" r:id="rId35" xr:uid="{B8241913-2A5E-4DB0-9873-AC74EC771BC3}"/>
+    <hyperlink ref="L7" r:id="rId36" xr:uid="{F95158DB-9593-4CF7-9172-F171351193DA}"/>
+    <hyperlink ref="M7" r:id="rId37" xr:uid="{6D4D8DF1-C19E-4230-BE24-9605580DAD56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1554,24 +1594,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Test Script on ComputerExecution.java and Excel Data
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143B54FB-3027-4E48-B505-EF8E9D1F4C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="77">
   <si>
     <t>TestCase</t>
   </si>
@@ -143,12 +142,6 @@
   </si>
   <si>
     <t>Shabadi</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>kattriguppe</t>
   </si>
   <si>
     <t>GiftcardsExceution.Giftcards</t>
@@ -259,8 +252,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,27 +470,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,24 +504,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,14 +679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
     <col min="2" max="3" width="29.33203125" customWidth="1"/>
@@ -757,7 +714,7 @@
     <col min="26" max="26" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" s="4" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,13 +722,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -850,7 +807,7 @@
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="8" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -904,7 +861,7 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" s="8" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -958,7 +915,7 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" s="8" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1046,80 +1003,80 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45">
       <c r="A5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="D5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="H5" s="11" t="s">
         <v>40</v>
       </c>
       <c r="I5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="13">
-        <v>560085</v>
-      </c>
-      <c r="N5" s="13">
-        <v>9019139736</v>
+      <c r="M5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="O5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z5" s="11">
+      <c r="P5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="7">
         <v>560085</v>
       </c>
-      <c r="AA5" s="11">
-        <v>9019139736</v>
-      </c>
+      <c r="U5" s="5">
+        <v>560085</v>
+      </c>
+      <c r="V5" s="5">
+        <v>9874563210</v>
+      </c>
+      <c r="W5" s="5">
+        <v>9874563210</v>
+      </c>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
@@ -1132,15 +1089,15 @@
       <c r="AK5" s="11"/>
       <c r="AL5" s="11"/>
     </row>
-    <row r="6" spans="1:45" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" s="16" customFormat="1">
       <c r="A6" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="13">
         <v>131099</v>
@@ -1155,19 +1112,19 @@
         <v>30</v>
       </c>
       <c r="H6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="M6" s="15">
         <v>560085</v>
@@ -1182,31 +1139,31 @@
         <v>30</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R6" s="13">
         <v>131099</v>
       </c>
       <c r="S6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="V6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="W6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="V6" s="13" t="s">
+      <c r="Y6" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="W6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y6" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="Z6" s="15">
         <v>560085</v>
@@ -1226,21 +1183,21 @@
       <c r="AK6" s="13"/>
       <c r="AL6" s="13"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45">
       <c r="A7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>30</v>
@@ -1249,22 +1206,22 @@
         <v>30</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>34</v>
@@ -1279,10 +1236,10 @@
         <v>35</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="T7" s="11">
         <v>560032</v>
@@ -1312,34 +1269,34 @@
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45">
       <c r="A8" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M8" s="13">
         <v>560085</v>
@@ -1376,21 +1333,21 @@
       <c r="AK8" s="11"/>
       <c r="AL8" s="11"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45">
       <c r="A9" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>30</v>
@@ -1399,22 +1356,22 @@
         <v>30</v>
       </c>
       <c r="H9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="M9" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="N9" s="11" t="s">
         <v>34</v>
@@ -1429,10 +1386,10 @@
         <v>35</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T9" s="11">
         <v>560096</v>
@@ -1462,21 +1419,21 @@
       <c r="AK9" s="11"/>
       <c r="AL9" s="11"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45">
       <c r="A10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>72</v>
-      </c>
       <c r="E10" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>30</v>
@@ -1485,22 +1442,22 @@
         <v>30</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N10" s="13" t="s">
         <v>34</v>
@@ -1515,10 +1472,10 @@
         <v>35</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="T10" s="11">
         <v>560085</v>
@@ -1550,43 +1507,43 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="J8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J10" r:id="rId11" display="pinkypriya@123gmail.com" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B6" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="Q6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="T6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="R10" r:id="rId16" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="R5" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="U5" r:id="rId18" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="V5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="W6" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B3" r:id="rId21" display="Bharathkumar@gmail.com" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B2" r:id="rId22" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D2" r:id="rId23" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C6" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C9" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E9" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="L9" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="M9" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C10" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E10" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L10" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="M10" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B7" r:id="rId33" xr:uid="{6F948A64-9E9A-489A-AAC1-1176D705DD43}"/>
-    <hyperlink ref="J7" r:id="rId34" display="tejaswinirty@gmail.com" xr:uid="{5A114D6A-FC17-4BA0-8D32-E28FC2B09E9A}"/>
-    <hyperlink ref="C7" r:id="rId35" xr:uid="{B8241913-2A5E-4DB0-9873-AC74EC771BC3}"/>
-    <hyperlink ref="L7" r:id="rId36" xr:uid="{F95158DB-9593-4CF7-9172-F171351193DA}"/>
-    <hyperlink ref="M7" r:id="rId37" xr:uid="{6D4D8DF1-C19E-4230-BE24-9605580DAD56}"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="J8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="J10" r:id="rId8" display="pinkypriya@123gmail.com"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="J6" r:id="rId10"/>
+    <hyperlink ref="Q6" r:id="rId11"/>
+    <hyperlink ref="T6" r:id="rId12"/>
+    <hyperlink ref="R10" r:id="rId13" display="PreetiLali@123"/>
+    <hyperlink ref="W6" r:id="rId14"/>
+    <hyperlink ref="B3" r:id="rId15" display="Bharathkumar@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId16" display="lalipreeti9@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId17" display="PreetiLali@123"/>
+    <hyperlink ref="C6" r:id="rId18"/>
+    <hyperlink ref="C9" r:id="rId19"/>
+    <hyperlink ref="E9" r:id="rId20"/>
+    <hyperlink ref="L9" r:id="rId21"/>
+    <hyperlink ref="M9" r:id="rId22"/>
+    <hyperlink ref="C10" r:id="rId23"/>
+    <hyperlink ref="E10" r:id="rId24"/>
+    <hyperlink ref="L10" r:id="rId25"/>
+    <hyperlink ref="M10" r:id="rId26"/>
+    <hyperlink ref="B7" r:id="rId27"/>
+    <hyperlink ref="J7" r:id="rId28" display="tejaswinirty@gmail.com"/>
+    <hyperlink ref="C7" r:id="rId29"/>
+    <hyperlink ref="L7" r:id="rId30"/>
+    <hyperlink ref="M7" r:id="rId31"/>
+    <hyperlink ref="B5" r:id="rId32"/>
+    <hyperlink ref="D5" r:id="rId33"/>
+    <hyperlink ref="M5" r:id="rId34"/>
+    <hyperlink ref="L5" r:id="rId35"/>
+    <hyperlink ref="E5" r:id="rId36"/>
+    <hyperlink ref="C5" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1594,24 +1551,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated ElectronicsExecution.java & ExcelDta
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEE36C2-E7CA-4388-9EC0-28CA338998D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
   <si>
     <t>TestCase</t>
   </si>
@@ -181,9 +180,6 @@
     <t>RT Nagar post office</t>
   </si>
   <si>
-    <t>ElectronicsExecution.checkout</t>
-  </si>
-  <si>
     <t>anilkumarsm28@gmail.com</t>
   </si>
   <si>
@@ -196,9 +192,6 @@
     <t>SM</t>
   </si>
   <si>
-    <t>kattreguppe</t>
-  </si>
-  <si>
     <t>vanigowdas54@gmail.com</t>
   </si>
   <si>
@@ -254,12 +247,15 @@
   </si>
   <si>
     <t>Assertion11</t>
+  </si>
+  <si>
+    <t>ElectronicsExecution.electronics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,23 +477,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -533,23 +512,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -725,11 +687,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -832,16 +794,16 @@
         <v>20</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -1326,52 +1288,74 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12" t="s">
+      <c r="E8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="K8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8" s="13">
-        <v>560085</v>
-      </c>
-      <c r="N8" s="13">
-        <v>7892540781</v>
+        <v>57</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="O8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
+      <c r="P8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" s="7">
+        <v>560085</v>
+      </c>
+      <c r="U8" s="7">
+        <v>560085</v>
+      </c>
+      <c r="V8" s="11">
+        <v>7892540781</v>
+      </c>
+      <c r="W8" s="11">
+        <v>7892540781</v>
+      </c>
       <c r="X8" s="11"/>
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
@@ -1390,19 +1374,19 @@
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>30</v>
@@ -1411,22 +1395,22 @@
         <v>30</v>
       </c>
       <c r="H9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="M9" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="N9" s="11" t="s">
         <v>34</v>
@@ -1441,10 +1425,10 @@
         <v>35</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T9" s="11">
         <v>560096</v>
@@ -1476,19 +1460,19 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="E10" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>30</v>
@@ -1497,22 +1481,22 @@
         <v>30</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N10" s="13" t="s">
         <v>34</v>
@@ -1527,10 +1511,10 @@
         <v>35</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="T10" s="11">
         <v>560085</v>
@@ -1562,45 +1546,48 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="J10" r:id="rId8" display="pinkypriya@123gmail.com" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="R10" r:id="rId9" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B3" r:id="rId10" display="Bharathkumar@gmail.com" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B2" r:id="rId11" display="lalipreeti9@gmail.com" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D2" r:id="rId12" display="PreetiLali@123" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="M9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L10" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="M10" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B7" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="J7" r:id="rId22" display="tejaswinirty@gmail.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="L7" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="M7" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D5" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="M5" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L5" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E5" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C5" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B6" r:id="rId32" xr:uid="{DBC6A9CA-0FDF-4B49-8983-F59179B0989C}"/>
-    <hyperlink ref="J6" r:id="rId33" display="achyutkembhavi4@gmail.com" xr:uid="{E39719EF-BDAD-40E8-B65E-68514FEE7F84}"/>
-    <hyperlink ref="C6" r:id="rId34" xr:uid="{0E0DDA79-7DBA-4FDD-8D89-C365560DEED7}"/>
-    <hyperlink ref="K6" r:id="rId35" display="achyutkembhavi4@gmail.com" xr:uid="{23D64729-AAE7-407B-A242-9FAF41683C28}"/>
-    <hyperlink ref="L6" r:id="rId36" xr:uid="{EED8C155-4A8A-47D3-9A75-BAC94BD05917}"/>
-    <hyperlink ref="M6" r:id="rId37" xr:uid="{07C98AF3-1AFD-4509-BE67-AFCA54701520}"/>
-    <hyperlink ref="Z6" r:id="rId38" xr:uid="{81847942-9F9A-46FD-9EF7-CD4CC6907618}"/>
-    <hyperlink ref="AA6" r:id="rId39" xr:uid="{69F57FAA-46DF-455C-9317-1A31407C8AE1}"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="D10" r:id="rId6"/>
+    <hyperlink ref="J10" r:id="rId7" display="pinkypriya@123gmail.com"/>
+    <hyperlink ref="R10" r:id="rId8" display="PreetiLali@123"/>
+    <hyperlink ref="B3" r:id="rId9" display="Bharathkumar@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId10" display="lalipreeti9@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId11" display="PreetiLali@123"/>
+    <hyperlink ref="C9" r:id="rId12"/>
+    <hyperlink ref="E9" r:id="rId13"/>
+    <hyperlink ref="L9" r:id="rId14"/>
+    <hyperlink ref="M9" r:id="rId15"/>
+    <hyperlink ref="C10" r:id="rId16"/>
+    <hyperlink ref="E10" r:id="rId17"/>
+    <hyperlink ref="L10" r:id="rId18"/>
+    <hyperlink ref="M10" r:id="rId19"/>
+    <hyperlink ref="B7" r:id="rId20"/>
+    <hyperlink ref="J7" r:id="rId21" display="tejaswinirty@gmail.com"/>
+    <hyperlink ref="C7" r:id="rId22"/>
+    <hyperlink ref="L7" r:id="rId23"/>
+    <hyperlink ref="M7" r:id="rId24"/>
+    <hyperlink ref="B5" r:id="rId25"/>
+    <hyperlink ref="D5" r:id="rId26"/>
+    <hyperlink ref="M5" r:id="rId27"/>
+    <hyperlink ref="L5" r:id="rId28"/>
+    <hyperlink ref="E5" r:id="rId29"/>
+    <hyperlink ref="C5" r:id="rId30"/>
+    <hyperlink ref="B6" r:id="rId31"/>
+    <hyperlink ref="J6" r:id="rId32" display="achyutkembhavi4@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId33"/>
+    <hyperlink ref="K6" r:id="rId34" display="achyutkembhavi4@gmail.com"/>
+    <hyperlink ref="L6" r:id="rId35"/>
+    <hyperlink ref="M6" r:id="rId36"/>
+    <hyperlink ref="Z6" r:id="rId37"/>
+    <hyperlink ref="AA6" r:id="rId38"/>
+    <hyperlink ref="C8" r:id="rId39"/>
+    <hyperlink ref="E8" r:id="rId40"/>
+    <hyperlink ref="L8" r:id="rId41"/>
+    <hyperlink ref="M8" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1608,7 +1595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1620,7 +1607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated Automation Script on ComputerExecution and Excel Data
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
@@ -129,9 +129,6 @@
     <t>Kattreguppe</t>
   </si>
   <si>
-    <t>ComputerExecution.checkout</t>
-  </si>
-  <si>
     <t>lalipreeti9@gmail.com</t>
   </si>
   <si>
@@ -250,13 +247,16 @@
   </si>
   <si>
     <t>ElectronicsExecution.electronics</t>
+  </si>
+  <si>
+    <t>ComputerExecution.computers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,7 +444,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -476,10 +476,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,7 +510,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -687,14 +685,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
     <col min="2" max="3" width="29.33203125" customWidth="1"/>
@@ -723,7 +721,7 @@
     <col min="27" max="27" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" s="4" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,13 +729,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -794,16 +792,16 @@
         <v>20</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -824,7 +822,7 @@
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="8" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -878,7 +876,7 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" s="8" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -932,7 +930,7 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" s="8" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1020,21 +1018,21 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45">
       <c r="A5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>30</v>
@@ -1043,22 +1041,22 @@
         <v>30</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="L5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>34</v>
@@ -1106,15 +1104,15 @@
       <c r="AK5" s="11"/>
       <c r="AL5" s="11"/>
     </row>
-    <row r="6" spans="1:45" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" s="16" customFormat="1">
       <c r="A6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="13">
         <v>131099</v>
@@ -1129,22 +1127,22 @@
         <v>30</v>
       </c>
       <c r="H6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="K6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>47</v>
-      </c>
       <c r="L6" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>34</v>
@@ -1177,16 +1175,16 @@
         <v>7829508059</v>
       </c>
       <c r="X6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="Y6" s="13" t="s">
+      <c r="AA6" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="Z6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA6" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="AB6" s="13"/>
       <c r="AC6" s="13"/>
@@ -1200,21 +1198,21 @@
       <c r="AK6" s="13"/>
       <c r="AL6" s="13"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45">
       <c r="A7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>30</v>
@@ -1223,22 +1221,22 @@
         <v>30</v>
       </c>
       <c r="H7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="L7" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>34</v>
@@ -1253,10 +1251,10 @@
         <v>35</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T7" s="11">
         <v>560032</v>
@@ -1286,21 +1284,21 @@
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45">
       <c r="A8" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>30</v>
@@ -1309,22 +1307,22 @@
         <v>30</v>
       </c>
       <c r="H8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>57</v>
-      </c>
       <c r="L8" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N8" s="13" t="s">
         <v>34</v>
@@ -1372,21 +1370,21 @@
       <c r="AK8" s="11"/>
       <c r="AL8" s="11"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45">
       <c r="A9" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="E9" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>30</v>
@@ -1395,22 +1393,22 @@
         <v>30</v>
       </c>
       <c r="H9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="L9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="M9" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="N9" s="11" t="s">
         <v>34</v>
@@ -1425,10 +1423,10 @@
         <v>35</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T9" s="11">
         <v>560096</v>
@@ -1458,21 +1456,21 @@
       <c r="AK9" s="11"/>
       <c r="AL9" s="11"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45">
       <c r="A10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>30</v>
@@ -1481,22 +1479,22 @@
         <v>30</v>
       </c>
       <c r="H10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="L10" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N10" s="13" t="s">
         <v>34</v>
@@ -1511,10 +1509,10 @@
         <v>35</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T10" s="11">
         <v>560085</v>
@@ -1595,24 +1593,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ApparelAndShoes module automation script is updated
</commit_message>
<xml_diff>
--- a/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
+++ b/DemoWebShopDWS_Taf/src/test/resources/ExcelData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="DemoWebShop" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
   <si>
     <t>TestCase</t>
   </si>
@@ -243,9 +243,6 @@
     <t>GM</t>
   </si>
   <si>
-    <t>Kattriguppe, BSK 3rd stage, Bangalore</t>
-  </si>
-  <si>
     <t>JewelryExecution.checkout</t>
   </si>
   <si>
@@ -253,13 +250,16 @@
   </si>
   <si>
     <t>Password_Assertion</t>
+  </si>
+  <si>
+    <t>Kamakya Layout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,7 +444,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -476,10 +476,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,7 +510,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -687,42 +685,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.21875" customWidth="1"/>
-    <col min="2" max="3" width="29.21875" customWidth="1"/>
-    <col min="4" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="25.5546875" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="20.5546875" customWidth="1"/>
-    <col min="14" max="14" width="25.5546875" customWidth="1"/>
-    <col min="15" max="15" width="23.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
+    <col min="14" max="14" width="25.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
     <col min="18" max="18" width="17" customWidth="1"/>
-    <col min="19" max="19" width="23.6640625" customWidth="1"/>
-    <col min="20" max="20" width="21.44140625" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" customWidth="1"/>
     <col min="21" max="21" width="24" customWidth="1"/>
-    <col min="22" max="22" width="24.5546875" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" customWidth="1"/>
     <col min="23" max="23" width="29" customWidth="1"/>
-    <col min="24" max="24" width="17.88671875" customWidth="1"/>
-    <col min="25" max="25" width="16.88671875" customWidth="1"/>
-    <col min="26" max="26" width="12.5546875" customWidth="1"/>
+    <col min="24" max="24" width="17.85546875" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" s="4" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,13 +728,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -815,7 +813,7 @@
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
     </row>
-    <row r="2" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" s="8" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -869,7 +867,7 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" s="8" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -923,7 +921,7 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" s="8" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -1011,7 +1009,7 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45">
       <c r="A5" s="11" t="s">
         <v>37</v>
       </c>
@@ -1097,7 +1095,7 @@
       <c r="AK5" s="11"/>
       <c r="AL5" s="11"/>
     </row>
-    <row r="6" spans="1:45" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" s="16" customFormat="1">
       <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
@@ -1191,7 +1189,7 @@
       <c r="AK6" s="13"/>
       <c r="AL6" s="13"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -1275,7 +1273,7 @@
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45">
       <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
@@ -1339,9 +1337,9 @@
       <c r="AK8" s="11"/>
       <c r="AL8" s="11"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45">
       <c r="A9" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>64</v>
@@ -1425,56 +1423,76 @@
       <c r="AK9" s="11"/>
       <c r="AL9" s="11"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45">
       <c r="A10" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="D10" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="E10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H10" s="11" t="s">
         <v>73</v>
       </c>
       <c r="I10" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="K10" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="M10" s="13">
-        <v>560085</v>
-      </c>
-      <c r="N10" s="13">
-        <v>7019561257</v>
+      <c r="M10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>34</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="T10" s="11">
+        <v>560085</v>
+      </c>
+      <c r="U10" s="11">
+        <v>560085</v>
+      </c>
+      <c r="V10" s="11">
+        <v>7019561257</v>
+      </c>
+      <c r="W10" s="11">
+        <v>7019561257</v>
+      </c>
       <c r="X10" s="11"/>
       <c r="Y10" s="11"/>
       <c r="Z10" s="11"/>
@@ -1503,12 +1521,12 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="B10" r:id="rId9"/>
     <hyperlink ref="D10" r:id="rId10"/>
-    <hyperlink ref="J10" r:id="rId11"/>
+    <hyperlink ref="J10" r:id="rId11" display="pinkypriya@123gmail.com"/>
     <hyperlink ref="B6" r:id="rId12"/>
     <hyperlink ref="J6" r:id="rId13"/>
     <hyperlink ref="Q6" r:id="rId14"/>
     <hyperlink ref="T6" r:id="rId15"/>
-    <hyperlink ref="R10" r:id="rId16"/>
+    <hyperlink ref="R10" r:id="rId16" display="PreetiLali@123"/>
     <hyperlink ref="R5" r:id="rId17"/>
     <hyperlink ref="U5" r:id="rId18" display="lalipreeti9@gmail.com"/>
     <hyperlink ref="V5" r:id="rId19"/>
@@ -1525,30 +1543,35 @@
     <hyperlink ref="E9" r:id="rId30"/>
     <hyperlink ref="L9" r:id="rId31"/>
     <hyperlink ref="M9" r:id="rId32"/>
+    <hyperlink ref="C10" r:id="rId33"/>
+    <hyperlink ref="E10" r:id="rId34"/>
+    <hyperlink ref="L10" r:id="rId35"/>
+    <hyperlink ref="M10" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>